<commit_message>
updated example data files
</commit_message>
<xml_diff>
--- a/braph2/workflows/MultiplexMRI/Group1_MRI_data_layer1.xlsx
+++ b/braph2/workflows/MultiplexMRI/Group1_MRI_data_layer1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kise-my.sharepoint.com/personal/anna_canal_garcia_ki_se/Documents/Dokument/PhD/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kise-my.sharepoint.com/personal/anna_canal_garcia_ki_se/Documents/Dokument/GitHub/Braph-2.0-Matlab/braph2/workflows/MultiplexMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_DE5CBECA8F79A8B36A3704F0FB5CC233402F0403" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{674DD5BD-6DC6-4579-923E-4CC50EFEDC87}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_DE5CBECA8F79A8B36A3704F0FB5CC233402F0403" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC60CB84-0ABF-422E-B5DD-9BA0ECFEA773}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>rFUS</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -285,13 +294,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,2310 +643,2376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BQ11"/>
+  <dimension ref="A1:BS11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2">
         <v>0.43000467331988951</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.65490382952172232</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>0.30418773603214089</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>0.52667284701719508</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.85281583958013496</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.92855475498937157</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>8.3196041485249506E-2</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>1.231882326299538E-2</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>0.73437268139693124</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>0.34827104292499189</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>0.60629234923606112</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>4.1349720367863552E-2</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>0.90755139008284391</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>0.41828706179123021</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>0.16479841204050441</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>0.23867716656580509</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>0.56437635684230192</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>0.62158162419461827</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>0.55269067918005388</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>0.39898694048000499</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>0.92218546800461509</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>0.1232104069668479</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>0.97273837743997216</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>0.70542202899954332</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>0.99100678369260309</v>
       </c>
-      <c r="AA2">
+      <c r="AC2">
         <v>0.23925577882956309</v>
       </c>
-      <c r="AB2">
+      <c r="AD2">
         <v>0.96090189896239186</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>0.13867758031090491</v>
       </c>
-      <c r="AD2">
+      <c r="AF2">
         <v>0.92970313839914109</v>
       </c>
-      <c r="AE2">
+      <c r="AG2">
         <v>5.9506122376415171E-2</v>
       </c>
-      <c r="AF2">
+      <c r="AH2">
         <v>0.21802412726988571</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>0.71766125973809347</v>
       </c>
-      <c r="AH2">
+      <c r="AJ2">
         <v>0.15941410875898721</v>
       </c>
-      <c r="AI2">
+      <c r="AK2">
         <v>0.95036743372042987</v>
       </c>
-      <c r="AJ2">
+      <c r="AL2">
         <v>0.98203432987225725</v>
       </c>
-      <c r="AK2">
+      <c r="AM2">
         <v>0.89545216583785869</v>
       </c>
-      <c r="AL2">
+      <c r="AN2">
         <v>0.5244673008231161</v>
       </c>
-      <c r="AM2">
+      <c r="AO2">
         <v>0.14012212772594329</v>
       </c>
-      <c r="AN2">
+      <c r="AP2">
         <v>0.50581298986444434</v>
       </c>
-      <c r="AO2">
+      <c r="AQ2">
         <v>0.9229222818266527</v>
       </c>
-      <c r="AP2">
+      <c r="AR2">
         <v>7.7744753307954717E-2</v>
       </c>
-      <c r="AQ2">
+      <c r="AS2">
         <v>0.61868879785417419</v>
       </c>
-      <c r="AR2">
+      <c r="AT2">
         <v>0.5161859969159468</v>
       </c>
-      <c r="AS2">
+      <c r="AU2">
         <v>0.32545525909588768</v>
       </c>
-      <c r="AT2">
+      <c r="AV2">
         <v>0.40519978938442869</v>
       </c>
-      <c r="AU2">
+      <c r="AW2">
         <v>0.87350043946810674</v>
       </c>
-      <c r="AV2">
+      <c r="AX2">
         <v>1.6879662476506518E-2</v>
       </c>
-      <c r="AW2">
+      <c r="AY2">
         <v>4.249403593969292E-2</v>
       </c>
-      <c r="AX2">
+      <c r="AZ2">
         <v>0.48190405343871923</v>
       </c>
-      <c r="AY2">
+      <c r="BA2">
         <v>6.0675739551639518E-2</v>
       </c>
-      <c r="AZ2">
+      <c r="BB2">
         <v>0.39031072355890117</v>
       </c>
-      <c r="BA2">
+      <c r="BC2">
         <v>0.47210354606356741</v>
       </c>
-      <c r="BB2">
+      <c r="BD2">
         <v>0.41198543387489311</v>
       </c>
-      <c r="BC2">
+      <c r="BE2">
         <v>7.1254265384862125E-2</v>
       </c>
-      <c r="BD2">
+      <c r="BF2">
         <v>0.87471472393533267</v>
       </c>
-      <c r="BE2">
+      <c r="BG2">
         <v>0.67205478991387424</v>
       </c>
-      <c r="BF2">
+      <c r="BH2">
         <v>0.24222247919932219</v>
       </c>
-      <c r="BG2">
+      <c r="BI2">
         <v>0.78312855366968492</v>
       </c>
-      <c r="BH2">
+      <c r="BJ2">
         <v>6.4149758231000553E-2</v>
       </c>
-      <c r="BI2">
+      <c r="BK2">
         <v>0.76229701708896425</v>
       </c>
-      <c r="BJ2">
+      <c r="BL2">
         <v>0.38958309706348948</v>
       </c>
-      <c r="BK2">
+      <c r="BM2">
         <v>0.25988113607571101</v>
       </c>
-      <c r="BL2">
+      <c r="BN2">
         <v>0.99814962289547826</v>
       </c>
-      <c r="BM2">
+      <c r="BO2">
         <v>4.7630965959818861E-2</v>
       </c>
-      <c r="BN2">
+      <c r="BP2">
         <v>0.21028982280731229</v>
       </c>
-      <c r="BO2">
+      <c r="BQ2">
         <v>0.40601853862067072</v>
       </c>
-      <c r="BP2">
+      <c r="BR2">
         <v>0.5091361989072466</v>
       </c>
-      <c r="BQ2">
+      <c r="BS2">
         <v>0.15830134285802569</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3">
         <v>0.31130251520430008</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>0.36142399295541372</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>0.96695450155887075</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>0.52798210883681473</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.42682426853342798</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.49222279273837632</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.5142892915413535</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0.77847986085368071</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.66089888545490805</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>0.50026181420327454</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>0.50672464072306878</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>0.15406839541068831</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>0.69575521467029777</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>0.64016726662689016</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>0.5394388283280529</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>0.23344384099262741</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>0.13100747478335481</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>0.56991390269946973</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>0.40273544723289278</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>0.99527308681590254</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>0.6587255236778804</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>0.28657693973997322</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>0.49351451041551608</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>0.30247054240336191</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>0.67362464247777998</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <v>0.13363474886096671</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>0.13643010613193049</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>0.75344417465214075</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>0.9743305510305007</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>0.9690099453266483</v>
       </c>
-      <c r="AF3">
+      <c r="AH3">
         <v>9.6031803940783478E-2</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>0.27506422637455458</v>
       </c>
-      <c r="AH3">
+      <c r="AJ3">
         <v>0.75912580792875284</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>0.351596311592271</v>
       </c>
-      <c r="AJ3">
+      <c r="AL3">
         <v>0.74933679832563083</v>
       </c>
-      <c r="AK3">
+      <c r="AM3">
         <v>0.37999868428055389</v>
       </c>
-      <c r="AL3">
+      <c r="AN3">
         <v>5.731513946717437E-2</v>
       </c>
-      <c r="AM3">
+      <c r="AO3">
         <v>4.713759530291628E-3</v>
       </c>
-      <c r="AN3">
+      <c r="AP3">
         <v>0.87084309738117482</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>0.93267171036511554</v>
       </c>
-      <c r="AP3">
+      <c r="AR3">
         <v>3.4688311856772243E-2</v>
       </c>
-      <c r="AQ3">
+      <c r="AS3">
         <v>0.8658638587797407</v>
       </c>
-      <c r="AR3">
+      <c r="AT3">
         <v>0.54390694139103413</v>
       </c>
-      <c r="AS3">
+      <c r="AU3">
         <v>0.39638524574983508</v>
       </c>
-      <c r="AT3">
+      <c r="AV3">
         <v>0.62711962936786059</v>
       </c>
-      <c r="AU3">
+      <c r="AW3">
         <v>0.23239385572624219</v>
       </c>
-      <c r="AV3">
+      <c r="AX3">
         <v>0.90471798941385106</v>
       </c>
-      <c r="AW3">
+      <c r="AY3">
         <v>0.70832664870522499</v>
       </c>
-      <c r="AX3">
+      <c r="AZ3">
         <v>0.1193420151732569</v>
       </c>
-      <c r="AY3">
+      <c r="BA3">
         <v>0.48001684957479979</v>
       </c>
-      <c r="AZ3">
+      <c r="BB3">
         <v>0.27596494067348931</v>
       </c>
-      <c r="BA3">
+      <c r="BC3">
         <v>0.35162530117506241</v>
       </c>
-      <c r="BB3">
+      <c r="BD3">
         <v>0.31036411710352357</v>
       </c>
-      <c r="BC3">
+      <c r="BE3">
         <v>8.1739608224289939E-2</v>
       </c>
-      <c r="BD3">
+      <c r="BF3">
         <v>3.7040193081189672E-2</v>
       </c>
-      <c r="BE3">
+      <c r="BG3">
         <v>0.26109052336350819</v>
       </c>
-      <c r="BF3">
+      <c r="BH3">
         <v>0.35127179951925502</v>
       </c>
-      <c r="BG3">
+      <c r="BI3">
         <v>0.51982501167378969</v>
       </c>
-      <c r="BH3">
+      <c r="BJ3">
         <v>0.42905966725695938</v>
       </c>
-      <c r="BI3">
+      <c r="BK3">
         <v>0.92379380859119653</v>
       </c>
-      <c r="BJ3">
+      <c r="BL3">
         <v>0.35465973518209237</v>
       </c>
-      <c r="BK3">
+      <c r="BM3">
         <v>0.18490468583970429</v>
       </c>
-      <c r="BL3">
+      <c r="BN3">
         <v>0.8628335784448159</v>
       </c>
-      <c r="BM3">
+      <c r="BO3">
         <v>0.1052640852082859</v>
       </c>
-      <c r="BN3">
+      <c r="BP3">
         <v>0.62448610604043575</v>
       </c>
-      <c r="BO3">
+      <c r="BQ3">
         <v>0.76269067461152185</v>
       </c>
-      <c r="BP3">
+      <c r="BR3">
         <v>7.8398039112830498E-2</v>
       </c>
-      <c r="BQ3">
+      <c r="BS3">
         <v>0.412105830579925</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4">
         <v>0.91359318452163385</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>0.2362056534429996</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.19150388628678011</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>3.9141851246586312E-2</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.1655251701422</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.160638727847396</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.62475539672400393</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>0.75139517502096487</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>0.96731706892733649</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>0.43933422727202143</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>0.39994831656054147</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>0.97616576096310015</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>0.31448150035227918</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>0.71886630322109824</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>9.4894166277128988E-2</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>0.34606143809454221</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>0.41336755140330611</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>0.96574145149372403</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>0.24428500155673821</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>3.6475360242983923E-2</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>0.69463325681208177</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>0.41602082641901278</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
         <v>2.849254792186906E-2</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>0.36557436778591368</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>0.78787905894382082</v>
       </c>
-      <c r="AA4">
+      <c r="AC4">
         <v>0.91792049296260481</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>0.26709676191506981</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>0.46080806127302248</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>0.95528414535518813</v>
       </c>
-      <c r="AE4">
+      <c r="AG4">
         <v>0.4096535855515262</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>0.74889782742817368</v>
       </c>
-      <c r="AG4">
+      <c r="AI4">
         <v>0.62785629176449997</v>
       </c>
-      <c r="AH4">
+      <c r="AJ4">
         <v>0.54859490919682052</v>
       </c>
-      <c r="AI4">
+      <c r="AK4">
         <v>8.3334716914112095E-2</v>
       </c>
-      <c r="AJ4">
+      <c r="AL4">
         <v>3.7814700053321881E-2</v>
       </c>
-      <c r="AK4">
+      <c r="AM4">
         <v>0.9624783582097225</v>
       </c>
-      <c r="AL4">
+      <c r="AN4">
         <v>0.12235041327576469</v>
       </c>
-      <c r="AM4">
+      <c r="AO4">
         <v>0.14951182565282939</v>
       </c>
-      <c r="AN4">
+      <c r="AP4">
         <v>2.389935764131235E-2</v>
       </c>
-      <c r="AO4">
+      <c r="AQ4">
         <v>0.87768950296441439</v>
       </c>
-      <c r="AP4">
+      <c r="AR4">
         <v>0.77305925431987088</v>
       </c>
-      <c r="AQ4">
+      <c r="AS4">
         <v>0.99022503673605222</v>
       </c>
-      <c r="AR4">
+      <c r="AT4">
         <v>0.91860109877131735</v>
       </c>
-      <c r="AS4">
+      <c r="AU4">
         <v>0.12313865191021391</v>
       </c>
-      <c r="AT4">
+      <c r="AV4">
         <v>0.49018202908146352</v>
       </c>
-      <c r="AU4">
+      <c r="AW4">
         <v>0.68869943186311489</v>
       </c>
-      <c r="AV4">
+      <c r="AX4">
         <v>0.4773958408560719</v>
       </c>
-      <c r="AW4">
+      <c r="AY4">
         <v>0.53900011853479257</v>
       </c>
-      <c r="AX4">
+      <c r="AZ4">
         <v>0.78821767721559111</v>
       </c>
-      <c r="AY4">
+      <c r="BA4">
         <v>0.26876477290787509</v>
       </c>
-      <c r="AZ4">
+      <c r="BB4">
         <v>0.62018792724499805</v>
       </c>
-      <c r="BA4">
+      <c r="BC4">
         <v>0.25017041311250487</v>
       </c>
-      <c r="BB4">
+      <c r="BD4">
         <v>0.91429011596005982</v>
       </c>
-      <c r="BC4">
+      <c r="BE4">
         <v>0.56171618589646899</v>
       </c>
-      <c r="BD4">
+      <c r="BF4">
         <v>8.4963357200987688E-2</v>
       </c>
-      <c r="BE4">
+      <c r="BG4">
         <v>6.7416836377950373E-2</v>
       </c>
-      <c r="BF4">
+      <c r="BH4">
         <v>0.28731953981688751</v>
       </c>
-      <c r="BG4">
+      <c r="BI4">
         <v>0.60268684587684151</v>
       </c>
-      <c r="BH4">
+      <c r="BJ4">
         <v>0.17704642119446981</v>
       </c>
-      <c r="BI4">
+      <c r="BK4">
         <v>0.28417102652555781</v>
       </c>
-      <c r="BJ4">
+      <c r="BL4">
         <v>0.51519438447982435</v>
       </c>
-      <c r="BK4">
+      <c r="BM4">
         <v>0.45787448000565512</v>
       </c>
-      <c r="BL4">
+      <c r="BN4">
         <v>0.6774215683274929</v>
       </c>
-      <c r="BM4">
+      <c r="BO4">
         <v>0.22474438547737499</v>
       </c>
-      <c r="BN4">
+      <c r="BP4">
         <v>0.63944518068272993</v>
       </c>
-      <c r="BO4">
+      <c r="BQ4">
         <v>0.505177670796081</v>
       </c>
-      <c r="BP4">
+      <c r="BR4">
         <v>0.1128492703111067</v>
       </c>
-      <c r="BQ4">
+      <c r="BS4">
         <v>6.667024361030538E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5">
         <v>8.1418585823363254E-2</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>0.1215605957648395</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>0.55420908911480915</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>0.39027651644156969</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.51846463051859071</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0.45720061998267802</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>0.89695912119364374</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0.32222724111743267</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>0.57644847711165703</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>0.72956488110604745</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>0.18109845108889869</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>0.65432879792858933</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>0.41145345128333027</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>0.31402878429251269</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>0.61589356006192275</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>0.9082846982229672</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>0.52174373077904612</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>0.1120699701515965</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>0.60226392029438902</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>0.72346524219945174</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>3.55928028414082E-2</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>0.89307843300985768</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>0.48236389880117891</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>0.27380140573789619</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>0.17252321722103689</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <v>0.2156178425498613</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>0.84571031928322193</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>0.97562468759328225</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>9.8983948710171799E-2</v>
       </c>
-      <c r="AE5">
+      <c r="AG5">
         <v>0.95101566200449317</v>
       </c>
-      <c r="AF5">
+      <c r="AH5">
         <v>0.73621350680180919</v>
       </c>
-      <c r="AG5">
+      <c r="AI5">
         <v>0.3415854477378325</v>
       </c>
-      <c r="AH5">
+      <c r="AJ5">
         <v>0.78174007724466255</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>0.58573438926259591</v>
       </c>
-      <c r="AJ5">
+      <c r="AL5">
         <v>4.2051122867598052E-2</v>
       </c>
-      <c r="AK5">
+      <c r="AM5">
         <v>0.95195265282894037</v>
       </c>
-      <c r="AL5">
+      <c r="AN5">
         <v>0.408719650779927</v>
       </c>
-      <c r="AM5">
+      <c r="AO5">
         <v>0.46542217474826442</v>
       </c>
-      <c r="AN5">
+      <c r="AP5">
         <v>0.73945514171133431</v>
       </c>
-      <c r="AO5">
+      <c r="AQ5">
         <v>0.6177122829314603</v>
       </c>
-      <c r="AP5">
+      <c r="AR5">
         <v>0.78537420157932714</v>
       </c>
-      <c r="AQ5">
+      <c r="AS5">
         <v>0.33480655921020991</v>
       </c>
-      <c r="AR5">
+      <c r="AT5">
         <v>0.54900681817430363</v>
       </c>
-      <c r="AS5">
+      <c r="AU5">
         <v>0.47744333281340789</v>
       </c>
-      <c r="AT5">
+      <c r="AV5">
         <v>0.84728535744226119</v>
       </c>
-      <c r="AU5">
+      <c r="AW5">
         <v>0.50326912638521737</v>
       </c>
-      <c r="AV5">
+      <c r="AX5">
         <v>0.48502496705981168</v>
       </c>
-      <c r="AW5">
+      <c r="AY5">
         <v>0.31877273870945172</v>
       </c>
-      <c r="AX5">
+      <c r="AZ5">
         <v>0.83878614045097011</v>
       </c>
-      <c r="AY5">
+      <c r="BA5">
         <v>0.46368584586993739</v>
       </c>
-      <c r="AZ5">
+      <c r="BB5">
         <v>0.31774734380543318</v>
       </c>
-      <c r="BA5">
+      <c r="BC5">
         <v>0.26867367354129829</v>
       </c>
-      <c r="BB5">
+      <c r="BD5">
         <v>0.90608470784621098</v>
       </c>
-      <c r="BC5">
+      <c r="BE5">
         <v>0.87061991503432901</v>
       </c>
-      <c r="BD5">
+      <c r="BF5">
         <v>2.3663201257982051E-2</v>
       </c>
-      <c r="BE5">
+      <c r="BG5">
         <v>0.71906026676634049</v>
       </c>
-      <c r="BF5">
+      <c r="BH5">
         <v>0.67775511037331382</v>
       </c>
-      <c r="BG5">
+      <c r="BI5">
         <v>0.69326230158318447</v>
       </c>
-      <c r="BH5">
+      <c r="BJ5">
         <v>0.88172812607387019</v>
       </c>
-      <c r="BI5">
+      <c r="BK5">
         <v>0.57326428670805851</v>
       </c>
-      <c r="BJ5">
+      <c r="BL5">
         <v>0.29755683593139037</v>
       </c>
-      <c r="BK5">
+      <c r="BM5">
         <v>0.45420506072196931</v>
       </c>
-      <c r="BL5">
+      <c r="BN5">
         <v>0.94120012392643682</v>
       </c>
-      <c r="BM5">
+      <c r="BO5">
         <v>0.93279989797389029</v>
       </c>
-      <c r="BN5">
+      <c r="BP5">
         <v>8.4552376079211955E-2</v>
       </c>
-      <c r="BO5">
+      <c r="BQ5">
         <v>0.21552043876632479</v>
       </c>
-      <c r="BP5">
+      <c r="BR5">
         <v>0.67342071260785386</v>
       </c>
-      <c r="BQ5">
+      <c r="BS5">
         <v>0.94267505080617453</v>
       </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6">
         <v>0.46809505230837589</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>1.7335137752102488E-2</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>0.1985621662546927</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>0.22059352318618969</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.46878005714078519</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>0.91467566304246128</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>0.92600368535503463</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>1.253590051809805E-2</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>0.80607157749226566</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>0.74547574292355134</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>0.40738984767193559</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>0.33176410016902719</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>7.4940219315248413E-2</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>4.30241943493479E-2</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>0.45425244289286371</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>0.44276128212054988</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>0.68597697900137178</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>0.37360417901570542</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>0.85883223506716477</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>0.46914646917509262</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>0.92030697553049412</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>0.77328662096177281</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>0.99639012918091874</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>0.95612527708617701</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>0.39177242946015067</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <v>0.30777252201222038</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>0.16599595126848879</v>
       </c>
-      <c r="AC6">
+      <c r="AE6">
         <v>0.77005605252989517</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>0.30919614972551968</v>
       </c>
-      <c r="AE6">
+      <c r="AG6">
         <v>0.49741486159234127</v>
       </c>
-      <c r="AF6">
+      <c r="AH6">
         <v>0.73712442788686616</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>0.98407017323778245</v>
       </c>
-      <c r="AH6">
+      <c r="AJ6">
         <v>0.90111175233696517</v>
       </c>
-      <c r="AI6">
+      <c r="AK6">
         <v>0.96830351865462749</v>
       </c>
-      <c r="AJ6">
+      <c r="AL6">
         <v>0.8038239254446915</v>
       </c>
-      <c r="AK6">
+      <c r="AM6">
         <v>0.73773996063428493</v>
       </c>
-      <c r="AL6">
+      <c r="AN6">
         <v>0.87134714541021374</v>
       </c>
-      <c r="AM6">
+      <c r="AO6">
         <v>0.32508399567208668</v>
       </c>
-      <c r="AN6">
+      <c r="AP6">
         <v>0.92179808387038598</v>
       </c>
-      <c r="AO6">
+      <c r="AQ6">
         <v>0.29818230631541942</v>
       </c>
-      <c r="AP6">
+      <c r="AR6">
         <v>0.7715467778643621</v>
       </c>
-      <c r="AQ6">
+      <c r="AS6">
         <v>0.91489789731314042</v>
       </c>
-      <c r="AR6">
+      <c r="AT6">
         <v>0.91002135967821751</v>
       </c>
-      <c r="AS6">
+      <c r="AU6">
         <v>0.92276543956028545</v>
       </c>
-      <c r="AT6">
+      <c r="AV6">
         <v>9.6526076130507454E-2</v>
       </c>
-      <c r="AU6">
+      <c r="AW6">
         <v>0.96510777087153288</v>
       </c>
-      <c r="AV6">
+      <c r="AX6">
         <v>0.23413541078711819</v>
       </c>
-      <c r="AW6">
+      <c r="AY6">
         <v>0.15550208549676001</v>
       </c>
-      <c r="AX6">
+      <c r="AZ6">
         <v>0.39091346422608009</v>
       </c>
-      <c r="AY6">
+      <c r="BA6">
         <v>0.49532032422672329</v>
       </c>
-      <c r="AZ6">
+      <c r="BB6">
         <v>0.23091513391664359</v>
       </c>
-      <c r="BA6">
+      <c r="BC6">
         <v>0.30239480035720651</v>
       </c>
-      <c r="BB6">
+      <c r="BD6">
         <v>0.56487164011003188</v>
       </c>
-      <c r="BC6">
+      <c r="BE6">
         <v>0.19770957678757561</v>
       </c>
-      <c r="BD6">
+      <c r="BF6">
         <v>0.59285535019177071</v>
       </c>
-      <c r="BE6">
+      <c r="BG6">
         <v>0.38100100415876142</v>
       </c>
-      <c r="BF6">
+      <c r="BH6">
         <v>0.26134451366035222</v>
       </c>
-      <c r="BG6">
+      <c r="BI6">
         <v>0.91902358689762442</v>
       </c>
-      <c r="BH6">
+      <c r="BJ6">
         <v>0.89116802191116606</v>
       </c>
-      <c r="BI6">
+      <c r="BK6">
         <v>0.41911979721314102</v>
       </c>
-      <c r="BJ6">
+      <c r="BL6">
         <v>7.5879380926815898E-2</v>
       </c>
-      <c r="BK6">
+      <c r="BM6">
         <v>0.40940828923191569</v>
       </c>
-      <c r="BL6">
+      <c r="BN6">
         <v>0.5938505003196155</v>
       </c>
-      <c r="BM6">
+      <c r="BO6">
         <v>0.40816610789569091</v>
       </c>
-      <c r="BN6">
+      <c r="BP6">
         <v>0.77228447335788142</v>
       </c>
-      <c r="BO6">
+      <c r="BQ6">
         <v>0.91320821357635695</v>
       </c>
-      <c r="BP6">
+      <c r="BR6">
         <v>0.49526737970147561</v>
       </c>
-      <c r="BQ6">
+      <c r="BS6">
         <v>0.21298349293023081</v>
       </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7">
         <v>0.62042601063254166</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>0.1955853476986672</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>0.49736845810114111</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>0.88286823276698279</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.72736013607179861</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>0.314158956620472</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.75001385642795659</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>0.1736376968888175</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>0.488365876215895</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>0.56302275716288519</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>2.3567343937837552E-2</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>0.95200917025492371</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>0.13953415858205159</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>0.83661140744303464</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>0.27475120831264849</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>0.62905976018360654</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>0.89204105383582954</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>5.5041514527765067E-2</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>0.72995234637766659</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>0.54206343213451147</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>4.2772483958663288E-2</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>0.71899365570194862</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <v>0.71081206868285329</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>0.52513930863661173</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>0.1702705174489246</v>
       </c>
-      <c r="AA7">
+      <c r="AC7">
         <v>0.46199495866666379</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>0.97588707187350354</v>
       </c>
-      <c r="AC7">
+      <c r="AE7">
         <v>0.64648439953514292</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>0.98617790353768164</v>
       </c>
-      <c r="AE7">
+      <c r="AG7">
         <v>0.41931323558853678</v>
       </c>
-      <c r="AF7">
+      <c r="AH7">
         <v>0.73034585626846749</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>0.28212020836174528</v>
       </c>
-      <c r="AH7">
+      <c r="AJ7">
         <v>8.6706686444696035E-2</v>
       </c>
-      <c r="AI7">
+      <c r="AK7">
         <v>0.2289765005450474</v>
       </c>
-      <c r="AJ7">
+      <c r="AL7">
         <v>0.40582009187610968</v>
       </c>
-      <c r="AK7">
+      <c r="AM7">
         <v>0.84726823293194731</v>
       </c>
-      <c r="AL7">
+      <c r="AN7">
         <v>0.40943127639203991</v>
       </c>
-      <c r="AM7">
+      <c r="AO7">
         <v>0.2544728327739787</v>
       </c>
-      <c r="AN7">
+      <c r="AP7">
         <v>7.9552719426108975E-2</v>
       </c>
-      <c r="AO7">
+      <c r="AQ7">
         <v>0.67622671736202256</v>
       </c>
-      <c r="AP7">
+      <c r="AR7">
         <v>0.53988908067644392</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7">
         <v>0.50495121886142258</v>
       </c>
-      <c r="AR7">
+      <c r="AT7">
         <v>0.2758480751510447</v>
       </c>
-      <c r="AS7">
+      <c r="AU7">
         <v>0.96827976157271722</v>
       </c>
-      <c r="AT7">
+      <c r="AV7">
         <v>0.31652931626620701</v>
       </c>
-      <c r="AU7">
+      <c r="AW7">
         <v>0.70364757007578216</v>
       </c>
-      <c r="AV7">
+      <c r="AX7">
         <v>0.3639083636900744</v>
       </c>
-      <c r="AW7">
+      <c r="AY7">
         <v>0.83577748219770076</v>
       </c>
-      <c r="AX7">
+      <c r="AZ7">
         <v>0.47246781681443012</v>
       </c>
-      <c r="AY7">
+      <c r="BA7">
         <v>0.40882169357377041</v>
       </c>
-      <c r="AZ7">
+      <c r="BB7">
         <v>0.76586140138896031</v>
       </c>
-      <c r="BA7">
+      <c r="BC7">
         <v>0.428055769680034</v>
       </c>
-      <c r="BB7">
+      <c r="BD7">
         <v>0.93181834570879851</v>
       </c>
-      <c r="BC7">
+      <c r="BE7">
         <v>0.47408197883241388</v>
       </c>
-      <c r="BD7">
+      <c r="BF7">
         <v>0.52442091125210988</v>
       </c>
-      <c r="BE7">
+      <c r="BG7">
         <v>0.26854607323531487</v>
       </c>
-      <c r="BF7">
+      <c r="BH7">
         <v>3.427155684986638E-2</v>
       </c>
-      <c r="BG7">
+      <c r="BI7">
         <v>0.87114643765532229</v>
       </c>
-      <c r="BH7">
+      <c r="BJ7">
         <v>0.83383091990748404</v>
       </c>
-      <c r="BI7">
+      <c r="BK7">
         <v>3.7328437585310681E-2</v>
       </c>
-      <c r="BJ7">
+      <c r="BL7">
         <v>0.11754323663490469</v>
       </c>
-      <c r="BK7">
+      <c r="BM7">
         <v>9.4948959507897501E-2</v>
       </c>
-      <c r="BL7">
+      <c r="BN7">
         <v>0.30847334305930058</v>
       </c>
-      <c r="BM7">
+      <c r="BO7">
         <v>0.80295517290099994</v>
       </c>
-      <c r="BN7">
+      <c r="BP7">
         <v>0.39214277077004123</v>
       </c>
-      <c r="BO7">
+      <c r="BQ7">
         <v>0.2800241417290652</v>
       </c>
-      <c r="BP7">
+      <c r="BR7">
         <v>0.1496215778493527</v>
       </c>
-      <c r="BQ7">
+      <c r="BS7">
         <v>0.56938450519629358</v>
       </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8">
         <v>7.0254307432461296E-3</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>0.27216114209191472</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>0.76388173326543984</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>3.1019469993909591E-2</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.1057015275584791</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>0.37730755011124462</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>0.37078211329222638</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>0.4759319874446305</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>0.31379081356785571</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>0.23132217899253449</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>0.57961944318729297</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>0.40193916778557059</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>0.68243188016507283</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>0.98468497346436301</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>0.99569358510133021</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>2.7720384511210169E-2</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>3.6172900922347151E-2</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>0.86099433412914561</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>0.94841297154016102</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <v>0.1089691240192865</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>0.74479372421770629</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <v>0.15309545900971011</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>0.35176417589684977</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>7.5235951417257474E-2</v>
       </c>
-      <c r="Z8">
+      <c r="AB8">
         <v>0.73667092708903503</v>
       </c>
-      <c r="AA8">
+      <c r="AC8">
         <v>0.8568505733471562</v>
       </c>
-      <c r="AB8">
+      <c r="AD8">
         <v>0.27648846098407248</v>
       </c>
-      <c r="AC8">
+      <c r="AE8">
         <v>0.978270966965192</v>
       </c>
-      <c r="AD8">
+      <c r="AF8">
         <v>0.13304080493601469</v>
       </c>
-      <c r="AE8">
+      <c r="AG8">
         <v>0.49953117516255419</v>
       </c>
-      <c r="AF8">
+      <c r="AH8">
         <v>0.63328538950346513</v>
       </c>
-      <c r="AG8">
+      <c r="AI8">
         <v>0.30326719397474577</v>
       </c>
-      <c r="AH8">
+      <c r="AJ8">
         <v>1.3964775811771021E-2</v>
       </c>
-      <c r="AI8">
+      <c r="AK8">
         <v>0.56158767492070016</v>
       </c>
-      <c r="AJ8">
+      <c r="AL8">
         <v>0.83597701290768167</v>
       </c>
-      <c r="AK8">
+      <c r="AM8">
         <v>0.57769497250900914</v>
       </c>
-      <c r="AL8">
+      <c r="AN8">
         <v>1.364447312134209E-2</v>
       </c>
-      <c r="AM8">
+      <c r="AO8">
         <v>0.43528396806419511</v>
       </c>
-      <c r="AN8">
+      <c r="AP8">
         <v>2.695372122637707E-2</v>
       </c>
-      <c r="AO8">
+      <c r="AQ8">
         <v>0.32877267864105819</v>
       </c>
-      <c r="AP8">
+      <c r="AR8">
         <v>8.2909915360955044E-2</v>
       </c>
-      <c r="AQ8">
+      <c r="AS8">
         <v>0.67920734329433241</v>
       </c>
-      <c r="AR8">
+      <c r="AT8">
         <v>0.81107798499262063</v>
       </c>
-      <c r="AS8">
+      <c r="AU8">
         <v>0.68765450293020369</v>
       </c>
-      <c r="AT8">
+      <c r="AV8">
         <v>0.22080828811272499</v>
       </c>
-      <c r="AU8">
+      <c r="AW8">
         <v>0.70228054052795874</v>
       </c>
-      <c r="AV8">
+      <c r="AX8">
         <v>0.1200671385206378</v>
       </c>
-      <c r="AW8">
+      <c r="AY8">
         <v>0.28708489877926441</v>
       </c>
-      <c r="AX8">
+      <c r="AZ8">
         <v>9.7897864823128788E-3</v>
       </c>
-      <c r="AY8">
+      <c r="BA8">
         <v>0.45290529916779582</v>
       </c>
-      <c r="AZ8">
+      <c r="BB8">
         <v>0.40597659607308417</v>
       </c>
-      <c r="BA8">
+      <c r="BC8">
         <v>4.1095940204996073E-2</v>
       </c>
-      <c r="BB8">
+      <c r="BD8">
         <v>0.44733968305340849</v>
       </c>
-      <c r="BC8">
+      <c r="BE8">
         <v>0.50295400251975375</v>
       </c>
-      <c r="BD8">
+      <c r="BF8">
         <v>0.34764477565129531</v>
       </c>
-      <c r="BE8">
+      <c r="BG8">
         <v>0.90283374217989976</v>
       </c>
-      <c r="BF8">
+      <c r="BH8">
         <v>0.93410712132062812</v>
       </c>
-      <c r="BG8">
+      <c r="BI8">
         <v>0.68482588093665786</v>
       </c>
-      <c r="BH8">
+      <c r="BJ8">
         <v>0.51809009131475015</v>
       </c>
-      <c r="BI8">
+      <c r="BK8">
         <v>0.51061692228363842</v>
       </c>
-      <c r="BJ8">
+      <c r="BL8">
         <v>0.2087501233813327</v>
       </c>
-      <c r="BK8">
+      <c r="BM8">
         <v>0.29664454846768668</v>
       </c>
-      <c r="BL8">
+      <c r="BN8">
         <v>0.39543251436017679</v>
       </c>
-      <c r="BM8">
+      <c r="BO8">
         <v>0.80130046877747885</v>
       </c>
-      <c r="BN8">
+      <c r="BP8">
         <v>0.41410915500828521</v>
       </c>
-      <c r="BO8">
+      <c r="BQ8">
         <v>0.17111442404718069</v>
       </c>
-      <c r="BP8">
+      <c r="BR8">
         <v>0.88164789630872331</v>
       </c>
-      <c r="BQ8">
+      <c r="BS8">
         <v>0.59188190608420166</v>
       </c>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9">
         <v>0.47140076417359378</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>0.52033736942877096</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>0.74163292691490668</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>0.8170566363719306</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>0.86824829958889138</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>0.35011090589153537</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>0.77334450782329955</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>0.47722232612819282</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>0.94914746558750751</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>0.16679509066113321</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>0.60287323861168263</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>0.11141879110903791</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>0.82894222519882654</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>0.98255817245449117</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>0.804808918777564</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>0.50477962802450405</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>5.5506829566872473E-2</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>0.83387699746163191</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>0.34847752638009277</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>0.298027102073124</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>0.4146876308812687</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>0.26197466905773442</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>6.4125934550006369E-2</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>0.73654981543469478</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>0.20429308880251759</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <v>0.11862393717375259</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>0.27575846825874051</v>
       </c>
-      <c r="AC9">
+      <c r="AE9">
         <v>0.66828533073183338</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>0.37654700909462951</v>
       </c>
-      <c r="AE9">
+      <c r="AG9">
         <v>0.86396255048927506</v>
       </c>
-      <c r="AF9">
+      <c r="AH9">
         <v>0.4191500463692962</v>
       </c>
-      <c r="AG9">
+      <c r="AI9">
         <v>0.65818880109712485</v>
       </c>
-      <c r="AH9">
+      <c r="AJ9">
         <v>0.97071443572032112</v>
       </c>
-      <c r="AI9">
+      <c r="AK9">
         <v>0.79645145905210224</v>
       </c>
-      <c r="AJ9">
+      <c r="AL9">
         <v>0.871583322105561</v>
       </c>
-      <c r="AK9">
+      <c r="AM9">
         <v>0.39375677598707398</v>
       </c>
-      <c r="AL9">
+      <c r="AN9">
         <v>0.25961933972632939</v>
       </c>
-      <c r="AM9">
+      <c r="AO9">
         <v>0.15107791303295451</v>
       </c>
-      <c r="AN9">
+      <c r="AP9">
         <v>0.40926090189945569</v>
       </c>
-      <c r="AO9">
+      <c r="AQ9">
         <v>0.21195139549424979</v>
       </c>
-      <c r="AP9">
+      <c r="AR9">
         <v>1.170345999169631E-2</v>
       </c>
-      <c r="AQ9">
+      <c r="AS9">
         <v>0.65111506496114402</v>
       </c>
-      <c r="AR9">
+      <c r="AT9">
         <v>0.35343491360052492</v>
       </c>
-      <c r="AS9">
+      <c r="AU9">
         <v>0.47984002473897441</v>
       </c>
-      <c r="AT9">
+      <c r="AV9">
         <v>0.35136256136032712</v>
       </c>
-      <c r="AU9">
+      <c r="AW9">
         <v>0.54340499425374922</v>
       </c>
-      <c r="AV9">
+      <c r="AX9">
         <v>0.7287771444869301</v>
       </c>
-      <c r="AW9">
+      <c r="AY9">
         <v>0.75300930636978969</v>
       </c>
-      <c r="AX9">
+      <c r="AZ9">
         <v>0.81645764260282472</v>
       </c>
-      <c r="AY9">
+      <c r="BA9">
         <v>0.77433178790573698</v>
       </c>
-      <c r="AZ9">
+      <c r="BB9">
         <v>0.7988244013046184</v>
       </c>
-      <c r="BA9">
+      <c r="BC9">
         <v>0.66693700361967356</v>
       </c>
-      <c r="BB9">
+      <c r="BD9">
         <v>0.1504931012859104</v>
       </c>
-      <c r="BC9">
+      <c r="BE9">
         <v>0.489618803390374</v>
       </c>
-      <c r="BD9">
+      <c r="BF9">
         <v>0.51821492258028334</v>
       </c>
-      <c r="BE9">
+      <c r="BG9">
         <v>0.85968204567374751</v>
       </c>
-      <c r="BF9">
+      <c r="BH9">
         <v>0.66202649989425133</v>
       </c>
-      <c r="BG9">
+      <c r="BI9">
         <v>0.247775764083742</v>
       </c>
-      <c r="BH9">
+      <c r="BJ9">
         <v>0.17800640849474539</v>
       </c>
-      <c r="BI9">
+      <c r="BK9">
         <v>1.531092119961097E-2</v>
       </c>
-      <c r="BJ9">
+      <c r="BL9">
         <v>0.87542684347476607</v>
       </c>
-      <c r="BK9">
+      <c r="BM9">
         <v>0.1664065020765039</v>
       </c>
-      <c r="BL9">
+      <c r="BN9">
         <v>0.67928992617466755</v>
       </c>
-      <c r="BM9">
+      <c r="BO9">
         <v>0.40969434901615492</v>
       </c>
-      <c r="BN9">
+      <c r="BP9">
         <v>0.90834426633215815</v>
       </c>
-      <c r="BO9">
+      <c r="BQ9">
         <v>0.59353912183065005</v>
       </c>
-      <c r="BP9">
+      <c r="BR9">
         <v>0.80885886920941141</v>
       </c>
-      <c r="BQ9">
+      <c r="BS9">
         <v>0.64889371458322498</v>
       </c>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10">
         <v>0.53487850648318458</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>0.82679133581138153</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>0.79159840974111362</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>0.96940123047692872</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>0.38556381522766942</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>0.11132873163615729</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.15259676207150499</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>0.16106688782272879</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>0.85649795528677208</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>0.62919359176109813</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>0.63262610576017886</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>0.4462853106792537</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>0.44674071698500178</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>0.15960091623082559</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>0.93449107331474257</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>0.21279780330656811</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>0.39003203352849708</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>2.4882557587322499E-2</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>0.99580907514367323</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>4.9795201898497947E-2</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>0.86911775768580968</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <v>0.47322329382263473</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
         <v>0.29947717479365699</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <v>0.77518537170127488</v>
       </c>
-      <c r="Z10">
+      <c r="AB10">
         <v>0.94659130201144193</v>
       </c>
-      <c r="AA10">
+      <c r="AC10">
         <v>0.24613677194912451</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <v>0.97113774263461683</v>
       </c>
-      <c r="AC10">
+      <c r="AE10">
         <v>0.49816044964513878</v>
       </c>
-      <c r="AD10">
+      <c r="AF10">
         <v>5.952143954560174E-2</v>
       </c>
-      <c r="AE10">
+      <c r="AG10">
         <v>0.21331642575785831</v>
       </c>
-      <c r="AF10">
+      <c r="AH10">
         <v>0.70762494025724199</v>
       </c>
-      <c r="AG10">
+      <c r="AI10">
         <v>0.113608671383817</v>
       </c>
-      <c r="AH10">
+      <c r="AJ10">
         <v>4.2364079924240849E-2</v>
       </c>
-      <c r="AI10">
+      <c r="AK10">
         <v>0.1466181526259486</v>
       </c>
-      <c r="AJ10">
+      <c r="AL10">
         <v>0.33582263069518209</v>
       </c>
-      <c r="AK10">
+      <c r="AM10">
         <v>0.21262792493949331</v>
       </c>
-      <c r="AL10">
+      <c r="AN10">
         <v>0.96573984873230168</v>
       </c>
-      <c r="AM10">
+      <c r="AO10">
         <v>0.96478311776166048</v>
       </c>
-      <c r="AN10">
+      <c r="AP10">
         <v>0.20845414181355471</v>
       </c>
-      <c r="AO10">
+      <c r="AQ10">
         <v>0.74530829835810386</v>
       </c>
-      <c r="AP10">
+      <c r="AR10">
         <v>0.91975510066558563</v>
       </c>
-      <c r="AQ10">
+      <c r="AS10">
         <v>0.85908467772634423</v>
       </c>
-      <c r="AR10">
+      <c r="AT10">
         <v>9.4716543936683606E-2</v>
       </c>
-      <c r="AS10">
+      <c r="AU10">
         <v>0.65221819060396513</v>
       </c>
-      <c r="AT10">
+      <c r="AV10">
         <v>0.54133214480609904</v>
       </c>
-      <c r="AU10">
+      <c r="AW10">
         <v>0.72461815481656489</v>
       </c>
-      <c r="AV10">
+      <c r="AX10">
         <v>0.83951881034086451</v>
       </c>
-      <c r="AW10">
+      <c r="AY10">
         <v>0.31580874809965342</v>
       </c>
-      <c r="AX10">
+      <c r="AZ10">
         <v>0.36707936001175367</v>
       </c>
-      <c r="AY10">
+      <c r="BA10">
         <v>0.7386948922954002</v>
       </c>
-      <c r="AZ10">
+      <c r="BB10">
         <v>6.7528962008871263E-2</v>
       </c>
-      <c r="BA10">
+      <c r="BC10">
         <v>0.88179124163483347</v>
       </c>
-      <c r="BB10">
+      <c r="BD10">
         <v>0.43035416611780258</v>
       </c>
-      <c r="BC10">
+      <c r="BE10">
         <v>3.6120796267764432E-2</v>
       </c>
-      <c r="BD10">
+      <c r="BF10">
         <v>0.51385037173521131</v>
       </c>
-      <c r="BE10">
+      <c r="BG10">
         <v>1.5870483332064981E-2</v>
       </c>
-      <c r="BF10">
+      <c r="BH10">
         <v>0.7135153948857037</v>
       </c>
-      <c r="BG10">
+      <c r="BI10">
         <v>5.415427395211514E-2</v>
       </c>
-      <c r="BH10">
+      <c r="BJ10">
         <v>0.9151034628700081</v>
       </c>
-      <c r="BI10">
+      <c r="BK10">
         <v>0.33880208038435189</v>
       </c>
-      <c r="BJ10">
+      <c r="BL10">
         <v>0.82472687569403347</v>
       </c>
-      <c r="BK10">
+      <c r="BM10">
         <v>6.1449791763464767E-2</v>
       </c>
-      <c r="BL10">
+      <c r="BN10">
         <v>0.45081671076230112</v>
       </c>
-      <c r="BM10">
+      <c r="BO10">
         <v>0.97151473001510524</v>
       </c>
-      <c r="BN10">
+      <c r="BP10">
         <v>0.47842343326365477</v>
       </c>
-      <c r="BO10">
+      <c r="BQ10">
         <v>0.68242763573583287</v>
       </c>
-      <c r="BP10">
+      <c r="BR10">
         <v>0.49106001073123817</v>
       </c>
-      <c r="BQ10">
+      <c r="BS10">
         <v>0.59525513631394</v>
       </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11">
         <v>0.63893515600733652</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>0.1556034832169336</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>0.1732958862530096</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>0.13893156081885699</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>0.91838469424567082</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>0.1850942306158361</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>0.89952698791038654</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>0.61131150203627738</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>0.88991293587417086</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>0.83752528306769924</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>0.63560069200340608</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>0.54778737588758764</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>0.73136208175697903</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>0.23652034081794729</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>0.31930217292117402</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>0.21259869171826659</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>0.34301636834653049</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>0.81887795069450886</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>1.499619125565255E-2</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <v>0.72319647968810274</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>0.4048559029922828</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <v>0.21969827940701009</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
         <v>0.15668694481086659</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <v>0.42640615317154151</v>
       </c>
-      <c r="Z11">
+      <c r="AB11">
         <v>0.77334659168633169</v>
       </c>
-      <c r="AA11">
+      <c r="AC11">
         <v>0.95596787965363994</v>
       </c>
-      <c r="AB11">
+      <c r="AD11">
         <v>0.93756355467156871</v>
       </c>
-      <c r="AC11">
+      <c r="AE11">
         <v>0.22763301515750631</v>
       </c>
-      <c r="AD11">
+      <c r="AF11">
         <v>0.86046177863154838</v>
       </c>
-      <c r="AE11">
+      <c r="AG11">
         <v>0.68516817723592427</v>
       </c>
-      <c r="AF11">
+      <c r="AH11">
         <v>0.139002986714059</v>
       </c>
-      <c r="AG11">
+      <c r="AI11">
         <v>6.3652712443995618E-2</v>
       </c>
-      <c r="AH11">
+      <c r="AJ11">
         <v>0.50943189151748114</v>
       </c>
-      <c r="AI11">
+      <c r="AK11">
         <v>0.65645444253711205</v>
       </c>
-      <c r="AJ11">
+      <c r="AL11">
         <v>0.89823032191121799</v>
       </c>
-      <c r="AK11">
+      <c r="AM11">
         <v>0.55785945704131945</v>
       </c>
-      <c r="AL11">
+      <c r="AN11">
         <v>0.42245119100712059</v>
       </c>
-      <c r="AM11">
+      <c r="AO11">
         <v>0.68200886013243056</v>
       </c>
-      <c r="AN11">
+      <c r="AP11">
         <v>0.1881671194388316</v>
       </c>
-      <c r="AO11">
+      <c r="AQ11">
         <v>0.45968242088359512</v>
       </c>
-      <c r="AP11">
+      <c r="AR11">
         <v>0.50630538021664517</v>
       </c>
-      <c r="AQ11">
+      <c r="AS11">
         <v>2.0310672093541871E-2</v>
       </c>
-      <c r="AR11">
+      <c r="AT11">
         <v>0.43491076178562382</v>
       </c>
-      <c r="AS11">
+      <c r="AU11">
         <v>0.14718224184997469</v>
       </c>
-      <c r="AT11">
+      <c r="AV11">
         <v>0.2778895106208259</v>
       </c>
-      <c r="AU11">
+      <c r="AW11">
         <v>0.81943502120083</v>
       </c>
-      <c r="AV11">
+      <c r="AX11">
         <v>0.47268201543791</v>
       </c>
-      <c r="AW11">
+      <c r="AY11">
         <v>0.99198443365116418</v>
       </c>
-      <c r="AX11">
+      <c r="AZ11">
         <v>0.30585694395043578</v>
       </c>
-      <c r="AY11">
+      <c r="BA11">
         <v>0.26967799026848649</v>
       </c>
-      <c r="AZ11">
+      <c r="BB11">
         <v>0.9261334429550202</v>
       </c>
-      <c r="BA11">
+      <c r="BC11">
         <v>0.48182530130587659</v>
       </c>
-      <c r="BB11">
+      <c r="BD11">
         <v>0.29645997660009599</v>
       </c>
-      <c r="BC11">
+      <c r="BE11">
         <v>0.1414973295403649</v>
       </c>
-      <c r="BD11">
+      <c r="BF11">
         <v>0.16457316911959979</v>
       </c>
-      <c r="BE11">
+      <c r="BG11">
         <v>0.58314902387765533</v>
       </c>
-      <c r="BF11">
+      <c r="BH11">
         <v>0.77033300246196923</v>
       </c>
-      <c r="BG11">
+      <c r="BI11">
         <v>0.19249160158548589</v>
       </c>
-      <c r="BH11">
+      <c r="BJ11">
         <v>0.42671337901952799</v>
       </c>
-      <c r="BI11">
+      <c r="BK11">
         <v>0.10286970627908699</v>
       </c>
-      <c r="BJ11">
+      <c r="BL11">
         <v>0.74079840461312263</v>
       </c>
-      <c r="BK11">
+      <c r="BM11">
         <v>0.6257865174977737</v>
       </c>
-      <c r="BL11">
+      <c r="BN11">
         <v>0.91657872951616071</v>
       </c>
-      <c r="BM11">
+      <c r="BO11">
         <v>0.23924975481196031</v>
       </c>
-      <c r="BN11">
+      <c r="BP11">
         <v>0.57498842591177435</v>
       </c>
-      <c r="BO11">
+      <c r="BQ11">
         <v>0.14154308638937449</v>
       </c>
-      <c r="BP11">
+      <c r="BR11">
         <v>0.99726171416815235</v>
       </c>
-      <c r="BQ11">
+      <c r="BS11">
         <v>0.47487126703314131</v>
       </c>
     </row>

</xml_diff>